<commit_message>
Add graphQl drive script
</commit_message>
<xml_diff>
--- a/Controller.xlsx
+++ b/Controller.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbinzayed\Desktop\FinalFramework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationFramework\AutomationAPI-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="898"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="898"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="1" r:id="rId1"/>
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
   <si>
     <t>Test Sheet Name</t>
   </si>
@@ -1279,7 +1279,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1343,6 +1343,20 @@
         <v>69</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1359,9 +1373,10 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1580,7 +1595,7 @@
     <col min="11" max="16384" width="8.7265625" style="7" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="17" customFormat="1" ht="56" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="17" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>37</v>
       </c>
@@ -1721,7 +1736,7 @@
     <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="56" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="42" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>